<commit_message>
Display data of last update
</commit_message>
<xml_diff>
--- a/app/data/EV_list_USA.xlsx
+++ b/app/data/EV_list_USA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="273">
   <si>
     <t xml:space="preserve">Make</t>
   </si>
@@ -442,10 +442,10 @@
     <t xml:space="preserve">USA 7</t>
   </si>
   <si>
+    <t xml:space="preserve">USA 8</t>
+  </si>
+  <si>
     <t xml:space="preserve">NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USA 8</t>
   </si>
   <si>
     <t xml:space="preserve">USA 9</t>
@@ -1500,7 +1500,7 @@
   <dimension ref="A1:K1039"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E88" activeCellId="0" sqref="E88"/>
+      <selection pane="topLeft" activeCell="E88" activeCellId="1" sqref="C9 E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6478,7 +6478,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6584,19 +6584,19 @@
       <c r="B9" s="25" t="n">
         <v>7</v>
       </c>
-      <c r="C9" s="25" t="s">
-        <v>138</v>
+      <c r="C9" s="25" t="n">
+        <v>67890</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B10" s="25" t="n">
         <v>8</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6607,7 +6607,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6618,7 +6618,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6629,7 +6629,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6640,7 +6640,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6651,7 +6651,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6681,7 +6681,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="C9 A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7337,7 +7337,7 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
+      <selection pane="topLeft" activeCell="K13" activeCellId="1" sqref="C9 K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7947,7 +7947,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="C9 H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8602,7 +8602,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="1" sqref="C9 C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8771,7 +8771,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="C9 B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Fixed negative values in plot
</commit_message>
<xml_diff>
--- a/app/data/EV_list_USA.xlsx
+++ b/app/data/EV_list_USA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cars" sheetId="1" state="visible" r:id="rId2"/>
@@ -805,13 +805,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="\$#,##0.00"/>
     <numFmt numFmtId="166" formatCode="[$$-1009]#,##0.00;[RED]\-[$$-1009]#,##0.00"/>
     <numFmt numFmtId="167" formatCode="0%"/>
     <numFmt numFmtId="168" formatCode="0.00%"/>
     <numFmt numFmtId="169" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="170" formatCode="0.00"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -995,7 +996,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1124,8 +1125,12 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -6462,7 +6467,7 @@
   </sheetPr>
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
     </sheetView>
   </sheetViews>
@@ -7747,8 +7752,8 @@
   </sheetPr>
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K34" activeCellId="0" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7771,9 +7776,10 @@
         <v>200</v>
       </c>
       <c r="B2" s="32" t="n">
-        <v>0.900660501981506</v>
-      </c>
-      <c r="D2" s="33"/>
+        <v>90.0660501981506</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="34"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="1"/>
@@ -7784,9 +7790,10 @@
         <v>201</v>
       </c>
       <c r="B3" s="32" t="n">
-        <v>1.21770145310436</v>
-      </c>
-      <c r="D3" s="33"/>
+        <v>121.770145310436</v>
+      </c>
+      <c r="C3" s="33"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
     </row>
@@ -7795,9 +7802,10 @@
         <v>202</v>
       </c>
       <c r="B4" s="32" t="n">
-        <v>1.22906208718626</v>
-      </c>
-      <c r="D4" s="33"/>
+        <v>122.906208718626</v>
+      </c>
+      <c r="C4" s="33"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
     </row>
@@ -7806,9 +7814,10 @@
         <v>203</v>
       </c>
       <c r="B5" s="32" t="n">
-        <v>0.912285336856011</v>
-      </c>
-      <c r="D5" s="33"/>
+        <v>91.2285336856011</v>
+      </c>
+      <c r="C5" s="33"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
     </row>
@@ -7817,9 +7826,10 @@
         <v>204</v>
       </c>
       <c r="B6" s="32" t="n">
-        <v>1.53025099075297</v>
-      </c>
-      <c r="D6" s="33"/>
+        <v>153.025099075297</v>
+      </c>
+      <c r="C6" s="33"/>
+      <c r="D6" s="34"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
     </row>
@@ -7828,9 +7838,10 @@
         <v>205</v>
       </c>
       <c r="B7" s="32" t="n">
-        <v>1.05310435931308</v>
-      </c>
-      <c r="D7" s="33"/>
+        <v>105.310435931308</v>
+      </c>
+      <c r="C7" s="33"/>
+      <c r="D7" s="34"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
     </row>
@@ -7839,9 +7850,10 @@
         <v>206</v>
       </c>
       <c r="B8" s="32" t="n">
-        <v>1.01902245706737</v>
-      </c>
-      <c r="D8" s="33"/>
+        <v>101.902245706737</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="34"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
     </row>
@@ -7850,9 +7862,10 @@
         <v>207</v>
       </c>
       <c r="B9" s="32" t="n">
-        <v>0.960105680317041</v>
-      </c>
-      <c r="D9" s="33"/>
+        <v>96.0105680317041</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="34"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
     </row>
@@ -7861,9 +7874,10 @@
         <v>208</v>
       </c>
       <c r="B10" s="32" t="n">
-        <v>1.03276089828269</v>
-      </c>
-      <c r="D10" s="33"/>
+        <v>103.276089828269</v>
+      </c>
+      <c r="C10" s="33"/>
+      <c r="D10" s="34"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
     </row>
@@ -7872,9 +7886,10 @@
         <v>209</v>
       </c>
       <c r="B11" s="32" t="n">
-        <v>0.965125495376486</v>
-      </c>
-      <c r="D11" s="33"/>
+        <v>96.5125495376486</v>
+      </c>
+      <c r="C11" s="33"/>
+      <c r="D11" s="34"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
     </row>
@@ -7883,9 +7898,10 @@
         <v>210</v>
       </c>
       <c r="B12" s="32" t="n">
-        <v>0.882959048877147</v>
-      </c>
-      <c r="D12" s="33"/>
+        <v>88.2959048877147</v>
+      </c>
+      <c r="C12" s="33"/>
+      <c r="D12" s="34"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
     </row>
@@ -7894,9 +7910,10 @@
         <v>211</v>
       </c>
       <c r="B13" s="32" t="n">
-        <v>1.2782034346103</v>
-      </c>
-      <c r="D13" s="33"/>
+        <v>127.82034346103</v>
+      </c>
+      <c r="C13" s="33"/>
+      <c r="D13" s="34"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
     </row>
@@ -7905,9 +7922,10 @@
         <v>212</v>
       </c>
       <c r="B14" s="32" t="n">
-        <v>1.09511228533686</v>
-      </c>
-      <c r="D14" s="33"/>
+        <v>109.511228533686</v>
+      </c>
+      <c r="C14" s="33"/>
+      <c r="D14" s="34"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
     </row>
@@ -7916,9 +7934,10 @@
         <v>213</v>
       </c>
       <c r="B15" s="32" t="n">
-        <v>1.03725231175694</v>
-      </c>
-      <c r="D15" s="33"/>
+        <v>103.725231175694</v>
+      </c>
+      <c r="C15" s="33"/>
+      <c r="D15" s="34"/>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
     </row>
@@ -7927,9 +7946,10 @@
         <v>214</v>
       </c>
       <c r="B16" s="32" t="n">
-        <v>0.969616908850727</v>
-      </c>
-      <c r="D16" s="33"/>
+        <v>96.9616908850727</v>
+      </c>
+      <c r="C16" s="33"/>
+      <c r="D16" s="34"/>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
     </row>
@@ -7938,9 +7958,10 @@
         <v>215</v>
       </c>
       <c r="B17" s="32" t="n">
-        <v>1.00211360634082</v>
-      </c>
-      <c r="D17" s="33"/>
+        <v>100.211360634082</v>
+      </c>
+      <c r="C17" s="33"/>
+      <c r="D17" s="34"/>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
     </row>
@@ -7949,9 +7970,10 @@
         <v>216</v>
       </c>
       <c r="B18" s="32" t="n">
-        <v>0.980184940554822</v>
-      </c>
-      <c r="D18" s="33"/>
+        <v>98.0184940554822</v>
+      </c>
+      <c r="C18" s="33"/>
+      <c r="D18" s="34"/>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
     </row>
@@ -7960,9 +7982,10 @@
         <v>217</v>
       </c>
       <c r="B19" s="32" t="n">
-        <v>0.922589167767503</v>
-      </c>
-      <c r="D19" s="33"/>
+        <v>92.2589167767503</v>
+      </c>
+      <c r="C19" s="33"/>
+      <c r="D19" s="34"/>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
     </row>
@@ -7971,9 +7994,10 @@
         <v>218</v>
       </c>
       <c r="B20" s="32" t="n">
-        <v>0.895376486129458</v>
-      </c>
-      <c r="D20" s="33"/>
+        <v>89.5376486129458</v>
+      </c>
+      <c r="C20" s="33"/>
+      <c r="D20" s="34"/>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
     </row>
@@ -7982,9 +8006,10 @@
         <v>219</v>
       </c>
       <c r="B21" s="32" t="n">
-        <v>1.01215323645971</v>
-      </c>
-      <c r="D21" s="33"/>
+        <v>101.215323645971</v>
+      </c>
+      <c r="C21" s="33"/>
+      <c r="D21" s="34"/>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
     </row>
@@ -7993,9 +8018,10 @@
         <v>220</v>
       </c>
       <c r="B22" s="32" t="n">
-        <v>0.970937912813738</v>
-      </c>
-      <c r="D22" s="33"/>
+        <v>97.0937912813738</v>
+      </c>
+      <c r="C22" s="33"/>
+      <c r="D22" s="34"/>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
     </row>
@@ -8004,9 +8030,10 @@
         <v>221</v>
       </c>
       <c r="B23" s="32" t="n">
-        <v>0.998414795244386</v>
-      </c>
-      <c r="D23" s="33"/>
+        <v>99.8414795244386</v>
+      </c>
+      <c r="C23" s="33"/>
+      <c r="D23" s="34"/>
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
     </row>
@@ -8015,9 +8042,10 @@
         <v>222</v>
       </c>
       <c r="B24" s="32" t="n">
-        <v>0.972787318361955</v>
-      </c>
-      <c r="D24" s="33"/>
+        <v>97.2787318361955</v>
+      </c>
+      <c r="C24" s="33"/>
+      <c r="D24" s="34"/>
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
     </row>
@@ -8026,9 +8054,10 @@
         <v>223</v>
       </c>
       <c r="B25" s="32" t="n">
-        <v>1.03091149273448</v>
-      </c>
-      <c r="D25" s="33"/>
+        <v>103.091149273448</v>
+      </c>
+      <c r="C25" s="33"/>
+      <c r="D25" s="34"/>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
     </row>
@@ -8037,9 +8066,10 @@
         <v>224</v>
       </c>
       <c r="B26" s="32" t="n">
-        <v>0.869749009247028</v>
-      </c>
-      <c r="D26" s="33"/>
+        <v>86.9749009247028</v>
+      </c>
+      <c r="C26" s="33"/>
+      <c r="D26" s="34"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
     </row>
@@ -8048,9 +8078,10 @@
         <v>225</v>
       </c>
       <c r="B27" s="32" t="n">
-        <v>0.963540290620872</v>
-      </c>
-      <c r="D27" s="33"/>
+        <v>96.3540290620872</v>
+      </c>
+      <c r="C27" s="33"/>
+      <c r="D27" s="34"/>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
     </row>
@@ -8059,9 +8090,10 @@
         <v>226</v>
       </c>
       <c r="B28" s="32" t="n">
-        <v>1.10911492734478</v>
-      </c>
-      <c r="D28" s="33"/>
+        <v>110.911492734478</v>
+      </c>
+      <c r="C28" s="33"/>
+      <c r="D28" s="34"/>
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
     </row>
@@ -8070,9 +8102,10 @@
         <v>227</v>
       </c>
       <c r="B29" s="32" t="n">
-        <v>1.01188903566711</v>
-      </c>
-      <c r="D29" s="33"/>
+        <v>101.188903566711</v>
+      </c>
+      <c r="C29" s="33"/>
+      <c r="D29" s="34"/>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
     </row>
@@ -8081,9 +8114,10 @@
         <v>228</v>
       </c>
       <c r="B30" s="32" t="n">
-        <v>1.33738441215324</v>
-      </c>
-      <c r="D30" s="33"/>
+        <v>133.738441215324</v>
+      </c>
+      <c r="C30" s="33"/>
+      <c r="D30" s="34"/>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
     </row>
@@ -8092,9 +8126,10 @@
         <v>229</v>
       </c>
       <c r="B31" s="32" t="n">
-        <v>0.985204755614267</v>
-      </c>
-      <c r="D31" s="33"/>
+        <v>98.5204755614267</v>
+      </c>
+      <c r="C31" s="33"/>
+      <c r="D31" s="34"/>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
     </row>
@@ -8103,9 +8138,10 @@
         <v>230</v>
       </c>
       <c r="B32" s="32" t="n">
-        <v>0.987318361955086</v>
-      </c>
-      <c r="D32" s="33"/>
+        <v>98.7318361955086</v>
+      </c>
+      <c r="C32" s="33"/>
+      <c r="D32" s="34"/>
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
     </row>
@@ -8114,9 +8150,10 @@
         <v>231</v>
       </c>
       <c r="B33" s="32" t="n">
-        <v>1.01373844121532</v>
-      </c>
-      <c r="D33" s="33"/>
+        <v>101.373844121532</v>
+      </c>
+      <c r="C33" s="33"/>
+      <c r="D33" s="34"/>
       <c r="E33" s="13"/>
       <c r="F33" s="13"/>
     </row>
@@ -8125,9 +8162,10 @@
         <v>232</v>
       </c>
       <c r="B34" s="32" t="n">
-        <v>1.03725231175694</v>
-      </c>
-      <c r="D34" s="33"/>
+        <v>103.725231175694</v>
+      </c>
+      <c r="C34" s="33"/>
+      <c r="D34" s="34"/>
       <c r="E34" s="13"/>
       <c r="F34" s="13"/>
     </row>
@@ -8136,9 +8174,10 @@
         <v>233</v>
       </c>
       <c r="B35" s="32" t="n">
-        <v>0.92443857331572</v>
-      </c>
-      <c r="D35" s="33"/>
+        <v>92.443857331572</v>
+      </c>
+      <c r="C35" s="33"/>
+      <c r="D35" s="34"/>
       <c r="E35" s="13"/>
       <c r="F35" s="13"/>
     </row>
@@ -8147,9 +8186,10 @@
         <v>234</v>
       </c>
       <c r="B36" s="32" t="n">
-        <v>1.04280052840159</v>
-      </c>
-      <c r="D36" s="33"/>
+        <v>104.280052840159</v>
+      </c>
+      <c r="C36" s="33"/>
+      <c r="D36" s="34"/>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
     </row>
@@ -8158,9 +8198,10 @@
         <v>235</v>
       </c>
       <c r="B37" s="32" t="n">
-        <v>0.945046235138705</v>
-      </c>
-      <c r="D37" s="33"/>
+        <v>94.5046235138705</v>
+      </c>
+      <c r="C37" s="33"/>
+      <c r="D37" s="34"/>
       <c r="E37" s="13"/>
       <c r="F37" s="13"/>
     </row>
@@ -8169,9 +8210,10 @@
         <v>236</v>
       </c>
       <c r="B38" s="32" t="n">
-        <v>0.987846763540291</v>
-      </c>
-      <c r="D38" s="33"/>
+        <v>98.7846763540291</v>
+      </c>
+      <c r="C38" s="33"/>
+      <c r="D38" s="34"/>
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
     </row>
@@ -8180,9 +8222,10 @@
         <v>237</v>
       </c>
       <c r="B39" s="32" t="n">
-        <v>1.23725231175694</v>
-      </c>
-      <c r="D39" s="33"/>
+        <v>123.725231175694</v>
+      </c>
+      <c r="C39" s="33"/>
+      <c r="D39" s="34"/>
       <c r="E39" s="13"/>
       <c r="F39" s="13"/>
     </row>
@@ -8191,9 +8234,10 @@
         <v>238</v>
       </c>
       <c r="B40" s="32" t="n">
-        <v>1.03751651254954</v>
-      </c>
-      <c r="D40" s="33"/>
+        <v>103.751651254954</v>
+      </c>
+      <c r="C40" s="33"/>
+      <c r="D40" s="34"/>
       <c r="E40" s="13"/>
       <c r="F40" s="13"/>
     </row>
@@ -8202,9 +8246,10 @@
         <v>239</v>
       </c>
       <c r="B41" s="32" t="n">
-        <v>0.997093791281374</v>
-      </c>
-      <c r="D41" s="33"/>
+        <v>99.7093791281374</v>
+      </c>
+      <c r="C41" s="33"/>
+      <c r="D41" s="34"/>
       <c r="E41" s="13"/>
       <c r="F41" s="13"/>
     </row>
@@ -8213,9 +8258,10 @@
         <v>240</v>
       </c>
       <c r="B42" s="32" t="n">
-        <v>0.898811096433289</v>
-      </c>
-      <c r="D42" s="33"/>
+        <v>89.8811096433289</v>
+      </c>
+      <c r="C42" s="33"/>
+      <c r="D42" s="34"/>
       <c r="E42" s="13"/>
       <c r="F42" s="13"/>
     </row>
@@ -8224,9 +8270,10 @@
         <v>241</v>
       </c>
       <c r="B43" s="32" t="n">
-        <v>1.03513870541612</v>
-      </c>
-      <c r="D43" s="33"/>
+        <v>103.513870541612</v>
+      </c>
+      <c r="C43" s="33"/>
+      <c r="D43" s="34"/>
       <c r="E43" s="13"/>
       <c r="F43" s="13"/>
     </row>
@@ -8235,9 +8282,10 @@
         <v>242</v>
       </c>
       <c r="B44" s="32" t="n">
-        <v>0.901717305151915</v>
-      </c>
-      <c r="D44" s="33"/>
+        <v>90.1717305151915</v>
+      </c>
+      <c r="C44" s="33"/>
+      <c r="D44" s="34"/>
       <c r="E44" s="13"/>
       <c r="F44" s="13"/>
     </row>
@@ -8246,9 +8294,10 @@
         <v>243</v>
       </c>
       <c r="B45" s="32" t="n">
-        <v>0.900660501981506</v>
-      </c>
-      <c r="D45" s="33"/>
+        <v>90.0660501981506</v>
+      </c>
+      <c r="C45" s="33"/>
+      <c r="D45" s="34"/>
       <c r="E45" s="13"/>
       <c r="F45" s="13"/>
     </row>
@@ -8257,9 +8306,10 @@
         <v>244</v>
       </c>
       <c r="B46" s="32" t="n">
-        <v>1.12470277410832</v>
-      </c>
-      <c r="D46" s="33"/>
+        <v>112.470277410832</v>
+      </c>
+      <c r="C46" s="33"/>
+      <c r="D46" s="34"/>
       <c r="E46" s="13"/>
       <c r="F46" s="13"/>
     </row>
@@ -8268,9 +8318,10 @@
         <v>245</v>
       </c>
       <c r="B47" s="32" t="n">
-        <v>1.00924702774108</v>
-      </c>
-      <c r="D47" s="33"/>
+        <v>100.924702774108</v>
+      </c>
+      <c r="C47" s="33"/>
+      <c r="D47" s="34"/>
       <c r="E47" s="13"/>
       <c r="F47" s="13"/>
     </row>
@@ -8279,9 +8330,10 @@
         <v>246</v>
       </c>
       <c r="B48" s="32" t="n">
-        <v>0.947952443857332</v>
-      </c>
-      <c r="D48" s="33"/>
+        <v>94.7952443857332</v>
+      </c>
+      <c r="C48" s="33"/>
+      <c r="D48" s="34"/>
       <c r="E48" s="13"/>
       <c r="F48" s="13"/>
     </row>
@@ -8290,9 +8342,10 @@
         <v>247</v>
       </c>
       <c r="B49" s="32" t="n">
-        <v>1.33157199471598</v>
-      </c>
-      <c r="D49" s="33"/>
+        <v>133.157199471598</v>
+      </c>
+      <c r="C49" s="33"/>
+      <c r="D49" s="34"/>
       <c r="E49" s="13"/>
       <c r="F49" s="13"/>
     </row>
@@ -8301,9 +8354,10 @@
         <v>248</v>
       </c>
       <c r="B50" s="32" t="n">
-        <v>0.958784676354029</v>
-      </c>
-      <c r="D50" s="33"/>
+        <v>95.8784676354029</v>
+      </c>
+      <c r="C50" s="33"/>
+      <c r="D50" s="34"/>
       <c r="E50" s="13"/>
       <c r="F50" s="13"/>
     </row>
@@ -8312,9 +8366,10 @@
         <v>249</v>
       </c>
       <c r="B51" s="32" t="n">
-        <v>0.957199471598415</v>
-      </c>
-      <c r="D51" s="33"/>
+        <v>95.7199471598415</v>
+      </c>
+      <c r="C51" s="33"/>
+      <c r="D51" s="34"/>
       <c r="E51" s="13"/>
       <c r="F51" s="13"/>
     </row>
@@ -8323,9 +8378,10 @@
         <v>250</v>
       </c>
       <c r="B52" s="32" t="n">
-        <v>1.0449141347424</v>
-      </c>
-      <c r="D52" s="33"/>
+        <v>104.49141347424</v>
+      </c>
+      <c r="C52" s="33"/>
+      <c r="D52" s="34"/>
       <c r="E52" s="13"/>
       <c r="F52" s="13"/>
       <c r="G52" s="13"/>
@@ -8338,6 +8394,7 @@
       <c r="B53" s="28" t="s">
         <v>252</v>
       </c>
+      <c r="C53" s="33"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -8386,7 +8443,7 @@
       <c r="H2" s="25"/>
       <c r="I2" s="25"/>
       <c r="J2" s="30"/>
-      <c r="K2" s="34"/>
+      <c r="K2" s="35"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="25" t="s">
@@ -8398,7 +8455,7 @@
       <c r="H3" s="25"/>
       <c r="I3" s="25"/>
       <c r="J3" s="30"/>
-      <c r="K3" s="34"/>
+      <c r="K3" s="35"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="25" t="s">
@@ -8410,7 +8467,7 @@
       <c r="H4" s="25"/>
       <c r="I4" s="25"/>
       <c r="J4" s="30"/>
-      <c r="K4" s="34"/>
+      <c r="K4" s="35"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="25" t="s">
@@ -8422,7 +8479,7 @@
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
       <c r="J5" s="30"/>
-      <c r="K5" s="34"/>
+      <c r="K5" s="35"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="25" t="s">
@@ -8434,7 +8491,7 @@
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
       <c r="J6" s="30"/>
-      <c r="K6" s="34"/>
+      <c r="K6" s="35"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="25" t="s">
@@ -8446,7 +8503,7 @@
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
       <c r="J7" s="30"/>
-      <c r="K7" s="34"/>
+      <c r="K7" s="35"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="25" t="s">
@@ -8458,7 +8515,7 @@
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
       <c r="J8" s="30"/>
-      <c r="K8" s="34"/>
+      <c r="K8" s="35"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="25" t="s">
@@ -8470,7 +8527,7 @@
       <c r="H9" s="25"/>
       <c r="I9" s="25"/>
       <c r="J9" s="30"/>
-      <c r="K9" s="34"/>
+      <c r="K9" s="35"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="25" t="s">
@@ -8482,7 +8539,7 @@
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
       <c r="J10" s="30"/>
-      <c r="K10" s="34"/>
+      <c r="K10" s="35"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="25" t="s">
@@ -8494,7 +8551,7 @@
       <c r="H11" s="25"/>
       <c r="I11" s="25"/>
       <c r="J11" s="30"/>
-      <c r="K11" s="34"/>
+      <c r="K11" s="35"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="25" t="s">
@@ -8506,7 +8563,7 @@
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
       <c r="J12" s="30"/>
-      <c r="K12" s="34"/>
+      <c r="K12" s="35"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="25" t="s">
@@ -8529,7 +8586,7 @@
       <c r="H14" s="25"/>
       <c r="I14" s="25"/>
       <c r="J14" s="30"/>
-      <c r="K14" s="34"/>
+      <c r="K14" s="35"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="25" t="s">
@@ -8541,7 +8598,7 @@
       <c r="H15" s="25"/>
       <c r="I15" s="25"/>
       <c r="J15" s="30"/>
-      <c r="K15" s="34"/>
+      <c r="K15" s="35"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="25" t="s">
@@ -8553,7 +8610,7 @@
       <c r="H16" s="25"/>
       <c r="I16" s="25"/>
       <c r="J16" s="30"/>
-      <c r="K16" s="34"/>
+      <c r="K16" s="35"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="25" t="s">
@@ -8565,7 +8622,7 @@
       <c r="H17" s="25"/>
       <c r="I17" s="25"/>
       <c r="J17" s="30"/>
-      <c r="K17" s="34"/>
+      <c r="K17" s="35"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="25" t="s">
@@ -8577,7 +8634,7 @@
       <c r="H18" s="25"/>
       <c r="I18" s="25"/>
       <c r="J18" s="30"/>
-      <c r="K18" s="34"/>
+      <c r="K18" s="35"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="25" t="s">
@@ -8589,7 +8646,7 @@
       <c r="H19" s="25"/>
       <c r="I19" s="25"/>
       <c r="J19" s="30"/>
-      <c r="K19" s="34"/>
+      <c r="K19" s="35"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="25" t="s">
@@ -8601,7 +8658,7 @@
       <c r="H20" s="25"/>
       <c r="I20" s="25"/>
       <c r="J20" s="30"/>
-      <c r="K20" s="34"/>
+      <c r="K20" s="35"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="25" t="s">
@@ -8613,7 +8670,7 @@
       <c r="H21" s="25"/>
       <c r="I21" s="25"/>
       <c r="J21" s="30"/>
-      <c r="K21" s="34"/>
+      <c r="K21" s="35"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="25" t="s">
@@ -8625,7 +8682,7 @@
       <c r="H22" s="25"/>
       <c r="I22" s="25"/>
       <c r="J22" s="30"/>
-      <c r="K22" s="34"/>
+      <c r="K22" s="35"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="25" t="s">
@@ -8637,7 +8694,7 @@
       <c r="H23" s="25"/>
       <c r="I23" s="25"/>
       <c r="J23" s="30"/>
-      <c r="K23" s="34"/>
+      <c r="K23" s="35"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="25" t="s">
@@ -8649,7 +8706,7 @@
       <c r="H24" s="25"/>
       <c r="I24" s="25"/>
       <c r="J24" s="30"/>
-      <c r="K24" s="34"/>
+      <c r="K24" s="35"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="25" t="s">
@@ -8661,7 +8718,7 @@
       <c r="H25" s="25"/>
       <c r="I25" s="25"/>
       <c r="J25" s="30"/>
-      <c r="K25" s="34"/>
+      <c r="K25" s="35"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="25" t="s">
@@ -8673,7 +8730,7 @@
       <c r="H26" s="25"/>
       <c r="I26" s="25"/>
       <c r="J26" s="30"/>
-      <c r="K26" s="34"/>
+      <c r="K26" s="35"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="25" t="s">
@@ -8685,7 +8742,7 @@
       <c r="H27" s="25"/>
       <c r="I27" s="25"/>
       <c r="J27" s="30"/>
-      <c r="K27" s="34"/>
+      <c r="K27" s="35"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="25" t="s">
@@ -8697,7 +8754,7 @@
       <c r="H28" s="25"/>
       <c r="I28" s="25"/>
       <c r="J28" s="30"/>
-      <c r="K28" s="34"/>
+      <c r="K28" s="35"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="25" t="s">
@@ -8709,7 +8766,7 @@
       <c r="H29" s="25"/>
       <c r="I29" s="25"/>
       <c r="J29" s="30"/>
-      <c r="K29" s="34"/>
+      <c r="K29" s="35"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="25" t="s">
@@ -8721,7 +8778,7 @@
       <c r="H30" s="25"/>
       <c r="I30" s="25"/>
       <c r="J30" s="30"/>
-      <c r="K30" s="34"/>
+      <c r="K30" s="35"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="25" t="s">
@@ -8733,7 +8790,7 @@
       <c r="H31" s="25"/>
       <c r="I31" s="25"/>
       <c r="J31" s="30"/>
-      <c r="K31" s="34"/>
+      <c r="K31" s="35"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="25" t="s">
@@ -8745,7 +8802,7 @@
       <c r="H32" s="25"/>
       <c r="I32" s="25"/>
       <c r="J32" s="30"/>
-      <c r="K32" s="34"/>
+      <c r="K32" s="35"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="25" t="s">
@@ -8757,7 +8814,7 @@
       <c r="H33" s="25"/>
       <c r="I33" s="25"/>
       <c r="J33" s="30"/>
-      <c r="K33" s="34"/>
+      <c r="K33" s="35"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="25" t="s">
@@ -8769,7 +8826,7 @@
       <c r="H34" s="25"/>
       <c r="I34" s="25"/>
       <c r="J34" s="30"/>
-      <c r="K34" s="34"/>
+      <c r="K34" s="35"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="25" t="s">
@@ -8781,7 +8838,7 @@
       <c r="H35" s="25"/>
       <c r="I35" s="25"/>
       <c r="J35" s="30"/>
-      <c r="K35" s="34"/>
+      <c r="K35" s="35"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="25" t="s">
@@ -8793,7 +8850,7 @@
       <c r="H36" s="25"/>
       <c r="I36" s="25"/>
       <c r="J36" s="30"/>
-      <c r="K36" s="34"/>
+      <c r="K36" s="35"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="25" t="s">
@@ -8805,7 +8862,7 @@
       <c r="H37" s="25"/>
       <c r="I37" s="25"/>
       <c r="J37" s="30"/>
-      <c r="K37" s="34"/>
+      <c r="K37" s="35"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="25" t="s">
@@ -8817,7 +8874,7 @@
       <c r="H38" s="25"/>
       <c r="I38" s="25"/>
       <c r="J38" s="30"/>
-      <c r="K38" s="34"/>
+      <c r="K38" s="35"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="25" t="s">
@@ -8829,7 +8886,7 @@
       <c r="H39" s="25"/>
       <c r="I39" s="25"/>
       <c r="J39" s="30"/>
-      <c r="K39" s="34"/>
+      <c r="K39" s="35"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="25" t="s">
@@ -8841,7 +8898,7 @@
       <c r="H40" s="25"/>
       <c r="I40" s="25"/>
       <c r="J40" s="30"/>
-      <c r="K40" s="34"/>
+      <c r="K40" s="35"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="25" t="s">
@@ -8853,7 +8910,7 @@
       <c r="H41" s="25"/>
       <c r="I41" s="25"/>
       <c r="J41" s="30"/>
-      <c r="K41" s="34"/>
+      <c r="K41" s="35"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="25" t="s">
@@ -8865,7 +8922,7 @@
       <c r="H42" s="25"/>
       <c r="I42" s="25"/>
       <c r="J42" s="30"/>
-      <c r="K42" s="34"/>
+      <c r="K42" s="35"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="25" t="s">
@@ -8877,7 +8934,7 @@
       <c r="H43" s="25"/>
       <c r="I43" s="25"/>
       <c r="J43" s="30"/>
-      <c r="K43" s="34"/>
+      <c r="K43" s="35"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="25" t="s">
@@ -8889,7 +8946,7 @@
       <c r="H44" s="25"/>
       <c r="I44" s="25"/>
       <c r="J44" s="30"/>
-      <c r="K44" s="34"/>
+      <c r="K44" s="35"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="25" t="s">
@@ -8901,7 +8958,7 @@
       <c r="H45" s="25"/>
       <c r="I45" s="25"/>
       <c r="J45" s="30"/>
-      <c r="K45" s="34"/>
+      <c r="K45" s="35"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="25" t="s">
@@ -8913,7 +8970,7 @@
       <c r="H46" s="25"/>
       <c r="I46" s="25"/>
       <c r="J46" s="30"/>
-      <c r="K46" s="34"/>
+      <c r="K46" s="35"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="25" t="s">
@@ -8925,7 +8982,7 @@
       <c r="H47" s="25"/>
       <c r="I47" s="25"/>
       <c r="J47" s="30"/>
-      <c r="K47" s="34"/>
+      <c r="K47" s="35"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="25" t="s">
@@ -8937,7 +8994,7 @@
       <c r="H48" s="25"/>
       <c r="I48" s="25"/>
       <c r="J48" s="30"/>
-      <c r="K48" s="34"/>
+      <c r="K48" s="35"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="25" t="s">
@@ -8949,7 +9006,7 @@
       <c r="H49" s="25"/>
       <c r="I49" s="25"/>
       <c r="J49" s="30"/>
-      <c r="K49" s="34"/>
+      <c r="K49" s="35"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="25" t="s">
@@ -8961,7 +9018,7 @@
       <c r="H50" s="25"/>
       <c r="I50" s="25"/>
       <c r="J50" s="30"/>
-      <c r="K50" s="34"/>
+      <c r="K50" s="35"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="25" t="s">
@@ -8973,7 +9030,7 @@
       <c r="H51" s="25"/>
       <c r="I51" s="25"/>
       <c r="J51" s="30"/>
-      <c r="K51" s="34"/>
+      <c r="K51" s="35"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="25" t="s">
@@ -8984,7 +9041,7 @@
       </c>
       <c r="I52" s="29"/>
       <c r="J52" s="30"/>
-      <c r="K52" s="34"/>
+      <c r="K52" s="35"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="28" t="s">
@@ -9022,10 +9079,10 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>256</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="36" t="s">
         <v>257</v>
       </c>
     </row>
@@ -9033,7 +9090,7 @@
       <c r="A2" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="36" t="n">
+      <c r="B2" s="37" t="n">
         <v>1195</v>
       </c>
     </row>
@@ -9041,7 +9098,7 @@
       <c r="A3" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="36" t="n">
+      <c r="B3" s="37" t="n">
         <v>1395</v>
       </c>
     </row>
@@ -9049,7 +9106,7 @@
       <c r="A4" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="36" t="n">
+      <c r="B4" s="37" t="n">
         <v>1995</v>
       </c>
     </row>
@@ -9057,7 +9114,7 @@
       <c r="A5" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="36" t="n">
+      <c r="B5" s="37" t="n">
         <v>1095</v>
       </c>
     </row>
@@ -9065,7 +9122,7 @@
       <c r="A6" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="36" t="n">
+      <c r="B6" s="37" t="n">
         <v>1115</v>
       </c>
     </row>
@@ -9073,7 +9130,7 @@
       <c r="A7" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="36" t="n">
+      <c r="B7" s="37" t="n">
         <v>1375</v>
       </c>
     </row>
@@ -9081,7 +9138,7 @@
       <c r="A8" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="36" t="n">
+      <c r="B8" s="37" t="n">
         <v>1165</v>
       </c>
     </row>
@@ -9089,7 +9146,7 @@
       <c r="A9" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="36" t="n">
+      <c r="B9" s="37" t="n">
         <v>1140</v>
       </c>
     </row>
@@ -9097,7 +9154,7 @@
       <c r="A10" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="36" t="n">
+      <c r="B10" s="37" t="n">
         <v>1200</v>
       </c>
     </row>
@@ -9105,13 +9162,13 @@
       <c r="A11" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="B11" s="36"/>
+      <c r="B11" s="37"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="36" t="n">
+      <c r="B12" s="37" t="n">
         <v>1350</v>
       </c>
     </row>
@@ -9119,7 +9176,7 @@
       <c r="A13" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="B13" s="36" t="n">
+      <c r="B13" s="37" t="n">
         <v>1295</v>
       </c>
     </row>
@@ -9127,7 +9184,7 @@
       <c r="A14" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="36" t="n">
+      <c r="B14" s="37" t="n">
         <v>1295</v>
       </c>
     </row>
@@ -9135,7 +9192,7 @@
       <c r="A15" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="B15" s="36" t="n">
+      <c r="B15" s="37" t="n">
         <v>1715</v>
       </c>
     </row>

</xml_diff>